<commit_message>
Added Passenger and Airplane classes, don't know if we'll need them
</commit_message>
<xml_diff>
--- a/AirplaneData.xlsx
+++ b/AirplaneData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joebo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D06A036-0A1C-474A-83E4-4C78D7B791BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1355A7-9616-423C-8240-01479D856E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8F84E47A-8E1E-4ED6-A33A-38B04A01B854}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Airplane Type</t>
   </si>
@@ -422,63 +422,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E754B7-FCDE-4C03-9A13-26A984AC8077}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>140</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
         <v>160</v>
       </c>
     </row>

</xml_diff>